<commit_message>
nodes size is variable regarding it's degree
</commit_message>
<xml_diff>
--- a/demo/public/data.xlsx
+++ b/demo/public/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="0" windowWidth="27765" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="6210" yWindow="0" windowWidth="27765" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,7 +859,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="F1:G1048576"/>
+      <selection activeCell="F2" sqref="F2:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
         <v>15</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -948,7 +948,7 @@
         <v>15</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -969,7 +969,7 @@
         <v>15</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -990,7 +990,7 @@
         <v>15</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1011,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1032,7 +1032,7 @@
         <v>15</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1053,7 +1053,7 @@
         <v>15</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1074,7 +1074,7 @@
         <v>15</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1095,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1116,7 +1116,7 @@
         <v>15</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1137,7 +1137,7 @@
         <v>15</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1158,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1179,7 +1179,7 @@
         <v>15</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1200,7 +1200,7 @@
         <v>15</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1221,7 +1221,7 @@
         <v>15</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1242,7 +1242,7 @@
         <v>15</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1263,7 +1263,7 @@
         <v>15</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1284,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1305,7 +1305,7 @@
         <v>15</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1326,7 +1326,7 @@
         <v>15</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1347,7 +1347,7 @@
         <v>15</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1368,7 +1368,7 @@
         <v>15</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1389,7 +1389,7 @@
         <v>15</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1410,7 +1410,7 @@
         <v>15</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1431,7 +1431,7 @@
         <v>15</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1452,7 +1452,7 @@
         <v>15</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1473,7 +1473,7 @@
         <v>15</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1494,7 +1494,7 @@
         <v>15</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1515,7 +1515,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1536,7 +1536,7 @@
         <v>15</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -1557,7 +1557,7 @@
         <v>15</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>